<commit_message>
add more stl files
</commit_message>
<xml_diff>
--- a/HyperRail/PCB Files/ESP32 GRBL Controller/BOM/BOM_PartType-ESP32 GRBL Controller.xlsx
+++ b/HyperRail/PCB Files/ESP32 GRBL Controller/BOM/BOM_PartType-ESP32 GRBL Controller.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorian Brusind\Documents\GitHub\PersonalProjects\HyperRail\PCB Files\ESP32 GRBL Controller\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C1FC8B-1E9F-47D6-87B1-8205989762B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EEAB8F7-F05C-4352-9A53-C13FC707EE01}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A0516F36-FDB0-4C8B-9ABE-913AF78349DF}"/>
+    <workbookView xWindow="8505" yWindow="4155" windowWidth="19170" windowHeight="10170" xr2:uid="{A0516F36-FDB0-4C8B-9ABE-913AF78349DF}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_PartType-ESP32 GRBL Control" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="131">
   <si>
     <t>Comment</t>
   </si>
@@ -108,9 +108,6 @@
     <t>CMP-150561-3</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>1uF</t>
   </si>
   <si>
@@ -409,6 +406,27 @@
   </si>
   <si>
     <t>LMZM23601V5SILR</t>
+  </si>
+  <si>
+    <t>CRGCQ0603J470R</t>
+  </si>
+  <si>
+    <t>RMCF0603FT4K70</t>
+  </si>
+  <si>
+    <t>1825910-6</t>
+  </si>
+  <si>
+    <t>SN74LVC3G14DCUT</t>
+  </si>
+  <si>
+    <t>ESP32-WROOM-32E (8MB)</t>
+  </si>
+  <si>
+    <t>C1206C104K5RAC7800</t>
+  </si>
+  <si>
+    <t>CL31B105KOFNNNE</t>
   </si>
 </sst>
 </file>
@@ -471,13 +489,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -794,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2748073F-6926-4075-8ADC-A61D5D6F2143}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,7 +916,7 @@
         <v>23</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>24</v>
+        <v>129</v>
       </c>
       <c r="G4" s="3">
         <v>2</v>
@@ -903,13 +924,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>22</v>
@@ -918,7 +939,7 @@
         <v>23</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>24</v>
+        <v>130</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -926,22 +947,22 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="G6" s="3">
         <v>2</v>
@@ -949,22 +970,22 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="G7" s="3">
         <v>1</v>
@@ -972,22 +993,22 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="G8" s="3">
         <v>6</v>
@@ -995,22 +1016,22 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="G9" s="3">
         <v>7</v>
@@ -1018,22 +1039,22 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>24</v>
+      <c r="F10" s="4">
+        <v>5040771891</v>
       </c>
       <c r="G10" s="3">
         <v>1</v>
@@ -1041,22 +1062,22 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="F11" s="2" t="s">
-        <v>24</v>
+        <v>128</v>
       </c>
       <c r="G11" s="3">
         <v>1</v>
@@ -1064,22 +1085,22 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="F12" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G12" s="3">
         <v>1</v>
@@ -1087,22 +1108,22 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="G13" s="3">
         <v>19</v>
@@ -1110,22 +1131,22 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="F14" s="2" t="s">
-        <v>24</v>
+        <v>125</v>
       </c>
       <c r="G14" s="3">
         <v>1</v>
@@ -1133,22 +1154,22 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="F15" s="2" t="s">
-        <v>24</v>
+        <v>124</v>
       </c>
       <c r="G15" s="3">
         <v>1</v>
@@ -1156,22 +1177,22 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="G16" s="3">
         <v>1</v>
@@ -1179,22 +1200,22 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>90</v>
-      </c>
       <c r="F17" s="2" t="s">
-        <v>24</v>
+        <v>126</v>
       </c>
       <c r="G17" s="3">
         <v>2</v>
@@ -1202,22 +1223,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="G18" s="3">
         <v>1</v>
@@ -1225,22 +1246,22 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="F19" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G19" s="3">
         <v>1</v>
@@ -1248,22 +1269,22 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="G20" s="3">
         <v>3</v>
@@ -1271,22 +1292,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="G21" s="3">
         <v>1</v>
@@ -1294,22 +1315,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>118</v>
-      </c>
       <c r="F22" s="2" t="s">
-        <v>24</v>
+        <v>127</v>
       </c>
       <c r="G22" s="3">
         <v>1</v>
@@ -1317,22 +1338,22 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>123</v>
-      </c>
       <c r="F23" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G23" s="3">
         <v>2</v>

</xml_diff>